<commit_message>
Update exemples iiif collection
</commit_message>
<xml_diff>
--- a/iiif/collection_iiif.xlsx
+++ b/iiif/collection_iiif.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca\Documents\GitHub\SHERLOCK\iiif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7578C6-68DB-4B14-8A30-23F7CEE3577E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF812FA6-E500-44C5-BEB3-274E40741FD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABDC5E25-0FA4-41BE-9150-9BDB7AE3A285}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>collection</t>
   </si>
@@ -69,9 +70,6 @@
     <t>Anne Piéjus</t>
   </si>
   <si>
-    <t>id de l'image*</t>
-  </si>
-  <si>
     <t>n° de page**</t>
   </si>
   <si>
@@ -100,13 +98,40 @@
   </si>
   <si>
     <t>lieu de publication**</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>GMG</t>
+  </si>
+  <si>
+    <t>40CM</t>
+  </si>
+  <si>
+    <t>id de l'image</t>
+  </si>
+  <si>
+    <t>1678-01_148</t>
+  </si>
+  <si>
+    <t>1678-01_149</t>
+  </si>
+  <si>
+    <t>40CM_1</t>
+  </si>
+  <si>
+    <t>40CM_2</t>
+  </si>
+  <si>
+    <t>40CM_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +158,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00000A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -178,14 +209,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F379C2-2FF4-4130-9DA9-93CB115680B5}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -520,86 +554,94 @@
     <col min="13" max="16384" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-    </row>
-    <row r="4" spans="1:12" s="7" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="4" spans="1:4" s="5" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +649,95 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBF2167-B86A-4BF9-A1E6-BD283645A530}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>